<commit_message>
fix:  structure of the DataTable was fixed
</commit_message>
<xml_diff>
--- a/base de datos demo.xlsx
+++ b/base de datos demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\Documents\GITHUB\Python Projects\Envio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C9FD309-C160-4FFA-9AA7-CD0769B324B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79997331-E881-452D-8489-9A184E522250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2064" windowWidth="18648" windowHeight="10896" xr2:uid="{718E276C-B919-44EE-B0BF-CF31C59B4DE6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>idContrato</t>
   </si>
@@ -74,7 +74,10 @@
     <t>995365458</t>
   </si>
   <si>
-    <t>kevinmacash@gmail.com</t>
+    <t>alexandermacash@gmail.com</t>
+  </si>
+  <si>
+    <t>9909</t>
   </si>
 </sst>
 </file>
@@ -128,13 +131,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -470,17 +472,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FD533AD-A574-4983-860A-7C6EDDEE1035}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="16.44140625" customWidth="1"/>
     <col min="3" max="3" width="21.6640625" customWidth="1"/>
-    <col min="4" max="4" width="24.33203125" customWidth="1"/>
+    <col min="4" max="4" width="27.5546875" customWidth="1"/>
     <col min="5" max="5" width="17.44140625" customWidth="1"/>
     <col min="6" max="6" width="13.6640625" customWidth="1"/>
   </cols>
@@ -553,7 +555,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>12</v>
@@ -564,15 +566,10 @@
       <c r="F4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C9" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{BE05AFB3-29AA-4FE7-83C3-156BB4032CF2}"/>
-    <hyperlink ref="D4" r:id="rId2" xr:uid="{5FD449C2-F41C-4FD3-A208-DE0549A95B1F}"/>
-    <hyperlink ref="D3" r:id="rId3" xr:uid="{61EA02AC-08F3-4BCC-AF0D-407235CB9ED9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix: Send emails was fixed
</commit_message>
<xml_diff>
--- a/base de datos demo.xlsx
+++ b/base de datos demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\Documents\GITHUB\Python Projects\Envio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79997331-E881-452D-8489-9A184E522250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA42E406-A1E4-497C-A4EB-DAC02DD0FD47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2064" windowWidth="18648" windowHeight="10896" xr2:uid="{718E276C-B919-44EE-B0BF-CF31C59B4DE6}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="18648" windowHeight="10896" xr2:uid="{718E276C-B919-44EE-B0BF-CF31C59B4DE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>idContrato</t>
   </si>
@@ -68,9 +68,6 @@
     <t xml:space="preserve">Armando </t>
   </si>
   <si>
-    <t>Alejandro Sani</t>
-  </si>
-  <si>
     <t>995365458</t>
   </si>
   <si>
@@ -78,6 +75,21 @@
   </si>
   <si>
     <t>9909</t>
+  </si>
+  <si>
+    <t>Italo Pilatasig</t>
+  </si>
+  <si>
+    <t>fxbricio7@gmail.com</t>
+  </si>
+  <si>
+    <t>bfabita@hotmail.es</t>
+  </si>
+  <si>
+    <t>984556639</t>
+  </si>
+  <si>
+    <t>David Flores</t>
   </si>
 </sst>
 </file>
@@ -472,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FD533AD-A574-4983-860A-7C6EDDEE1035}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -515,10 +527,10 @@
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="E2" s="3">
         <v>15.69</v>
@@ -535,10 +547,10 @@
         <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="E3" s="3">
         <v>123</v>
@@ -552,24 +564,45 @@
         <v>5050</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E4" s="3">
         <v>8.23</v>
       </c>
       <c r="F4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>5050</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="3">
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{BE05AFB3-29AA-4FE7-83C3-156BB4032CF2}"/>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{E69A8A1D-EF0C-4D2F-BEDF-720A5CA4906E}"/>
+    <hyperlink ref="D5" r:id="rId2" xr:uid="{7C27F2A9-F7B3-4FE0-814A-92F047014929}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>